<commit_message>
Scene structure and pass through of mouse and key events.
</commit_message>
<xml_diff>
--- a/data/events.xlsx
+++ b/data/events.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="8760" windowWidth="28800" windowHeight="12080" tabRatio="500"/>
+    <workbookView xWindow="5000" yWindow="5120" windowWidth="28800" windowHeight="12080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>main_title</t>
   </si>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,9 +407,6 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>